<commit_message>
add some ui page
</commit_message>
<xml_diff>
--- a/documents/database.xlsx
+++ b/documents/database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="108">
   <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -419,15 +419,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>个人中心首页列表页</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>登陆页</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>注册页</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9月8号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post创建</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post修改</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post点赞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment the post</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9月10号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9月8号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9月10号</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -614,16 +650,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1281,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:B25"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1319,7 +1355,7 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1337,7 +1373,7 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" ht="40.5">
-      <c r="A3" s="11"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
@@ -1353,7 +1389,7 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" ht="54">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="14" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1371,7 +1407,7 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" ht="94.5">
-      <c r="A5" s="11"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="3" t="s">
         <v>33</v>
       </c>
@@ -1387,7 +1423,7 @@
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" ht="27">
-      <c r="A6" s="11"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="3" t="s">
         <v>34</v>
       </c>
@@ -1403,7 +1439,7 @@
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="11"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="3" t="s">
         <v>30</v>
       </c>
@@ -1419,7 +1455,7 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="11"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="3" t="s">
         <v>31</v>
       </c>
@@ -1435,7 +1471,7 @@
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="11"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
@@ -1451,7 +1487,7 @@
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>76</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1469,7 +1505,7 @@
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="14"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="3" t="s">
         <v>31</v>
       </c>
@@ -1503,7 +1539,7 @@
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1519,7 +1555,7 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="11"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="3" t="s">
         <v>38</v>
       </c>
@@ -1533,7 +1569,7 @@
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="11"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="3" t="s">
         <v>39</v>
       </c>
@@ -1547,7 +1583,7 @@
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>73</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1591,50 +1627,153 @@
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="B20" s="1" t="s">
+      <c r="A20" s="12"/>
+      <c r="B20" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="12"/>
+      <c r="B21" s="3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="12"/>
+      <c r="B22" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="12"/>
+      <c r="B23" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="12"/>
+      <c r="B24" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="B22" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="B23" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="B24" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="B25" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="A25" s="12"/>
+      <c r="B25" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="12"/>
+      <c r="B26" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="12"/>
+      <c r="B27" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="12"/>
+      <c r="B28" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="13"/>
+      <c r="B29" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A9"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A19:A29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>